<commit_message>
Added another version of partslist with modules instead
</commit_message>
<xml_diff>
--- a/B.0 System Design/SAN_Project_Partslistv2.xlsx
+++ b/B.0 System Design/SAN_Project_Partslistv2.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ad1c0a53281c2ab/Documents/University/Studies/Sem 5/Sensors and Actuator Networks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ad1c0a53281c2ab/Documents/University/Studies/Sem 5/Sensors and Actuator Networks/Project/B.0 System Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{4B84344F-A1E2-4550-9753-47CC572F610C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0B14857-0F7C-4A8C-AB24-E8EA981A795E}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{4B84344F-A1E2-4550-9753-47CC572F610C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F53DA40F-B0E8-4F6D-8236-0A83CC0DEBEF}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
   <si>
     <t>Link</t>
   </si>
@@ -274,6 +274,18 @@
   </si>
   <si>
     <t>IDUINO</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Amphenol-SAA/PIOV008NRAA-100?qs=GedFDFLaBXFCaCiGvxFhnA%3D%3D</t>
+  </si>
+  <si>
+    <t>523-PIOV008NRAA-100</t>
+  </si>
+  <si>
+    <t>Amphenol-SAA</t>
+  </si>
+  <si>
+    <t>PIOV008NRAA-100</t>
   </si>
 </sst>
 </file>
@@ -698,6 +710,71 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -711,71 +788,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1084,62 +1096,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScale="131" zoomScaleNormal="100" zoomScalePageLayoutView="131" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScale="131" zoomScaleNormal="100" zoomScalePageLayoutView="131" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" customWidth="1"/>
-    <col min="10" max="10" width="55.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
-    <col min="20" max="20" width="9.42578125" customWidth="1"/>
-    <col min="21" max="21" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" customWidth="1"/>
+    <col min="10" max="10" width="55.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="20" max="20" width="9.44140625" customWidth="1"/>
+    <col min="21" max="21" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="61"/>
       <c r="C1" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="61"/>
       <c r="C2" s="21" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+    </row>
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1171,20 +1183,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>1</v>
       </c>
       <c r="B5" s="22">
         <v>1</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="46" t="s">
         <v>78</v>
       </c>
       <c r="F5" s="23" t="s">
@@ -1204,7 +1216,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -1214,10 +1226,10 @@
       <c r="C6" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="50" t="s">
         <v>73</v>
       </c>
       <c r="F6" s="27" t="s">
@@ -1237,7 +1249,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>3</v>
       </c>
@@ -1247,10 +1259,10 @@
       <c r="C7" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="66">
+      <c r="E7" s="49">
         <v>102010611</v>
       </c>
       <c r="F7" s="27" t="s">
@@ -1270,7 +1282,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -1303,7 +1315,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>5</v>
       </c>
@@ -1336,7 +1348,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>6</v>
       </c>
@@ -1369,7 +1381,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>7</v>
       </c>
@@ -1402,7 +1414,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>8</v>
       </c>
@@ -1435,7 +1447,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>9</v>
       </c>
@@ -1468,24 +1480,40 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>10</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="31"/>
+      <c r="B14" s="29">
+        <v>1</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="31">
+        <v>2.69</v>
+      </c>
       <c r="I14" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="37"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.69</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>11</v>
       </c>
@@ -1502,7 +1530,7 @@
       </c>
       <c r="J15" s="37"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>12</v>
       </c>
@@ -1519,7 +1547,7 @@
       </c>
       <c r="J16" s="37"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>13</v>
       </c>
@@ -1536,7 +1564,7 @@
       </c>
       <c r="J17" s="37"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>14</v>
       </c>
@@ -1553,7 +1581,7 @@
       </c>
       <c r="J18" s="37"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>15</v>
       </c>
@@ -1570,18 +1598,18 @@
       </c>
       <c r="J19" s="38"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G20" s="47" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G20" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="47"/>
+      <c r="H20" s="67"/>
       <c r="I20" s="13">
         <f>SUM(I5:I19)</f>
-        <v>59.81</v>
+        <v>62.5</v>
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>25</v>
       </c>
@@ -1589,103 +1617,103 @@
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="16"/>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="48"/>
+      <c r="H21" s="68"/>
       <c r="I21" s="11">
         <f>I20*0.19</f>
-        <v>11.363900000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="51" t="s">
+        <v>11.875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="52"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="55"/>
-      <c r="G22" s="48" t="s">
+      <c r="E22" s="64"/>
+      <c r="G22" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="48"/>
+      <c r="H22" s="68"/>
       <c r="I22" s="12">
         <f>I20*1.19</f>
-        <v>71.173900000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
+        <v>74.375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="54"/>
+      <c r="B23" s="53"/>
       <c r="C23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="58" t="s">
+      <c r="D23" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="59"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="53" t="s">
+      <c r="E23" s="57"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="54"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="58" t="s">
+      <c r="D24" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="59"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="s">
+      <c r="E24" s="57"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="54"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="58" t="s">
+      <c r="D25" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="59"/>
+      <c r="E25" s="57"/>
       <c r="H25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="54"/>
+      <c r="B26" s="53"/>
       <c r="C26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="58" t="s">
+      <c r="D26" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="59"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="s">
+      <c r="E26" s="57"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="57"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="39"/>
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="61"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E27" s="59"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="40" t="s">
         <v>46</v>
       </c>
@@ -1698,7 +1726,7 @@
       </c>
       <c r="E28" s="42"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
@@ -1710,7 +1738,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="2"/>
@@ -1722,7 +1750,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="2"/>
@@ -1734,7 +1762,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2"/>
@@ -1746,7 +1774,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="2"/>
@@ -1758,7 +1786,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1770,7 +1798,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2"/>
@@ -1782,7 +1810,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="2"/>
@@ -1796,6 +1824,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A27:B27"/>
@@ -1805,16 +1843,6 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Schematic and Pitch Prez Update
</commit_message>
<xml_diff>
--- a/B.0 System Design/SAN_Project_Partslistv2.xlsx
+++ b/B.0 System Design/SAN_Project_Partslistv2.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ad1c0a53281c2ab/Documents/University/Studies/Sem 5/Sensors and Actuator Networks/Project/B.0 System Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Projects\LoRaProject\B.0 System Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{4B84344F-A1E2-4550-9753-47CC572F610C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F53DA40F-B0E8-4F6D-8236-0A83CC0DEBEF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8C8760-17EF-41F0-85DA-B166EF18A4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="5" r:id="rId1"/>
@@ -736,12 +736,41 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -759,35 +788,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1096,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScale="131" zoomScaleNormal="100" zoomScalePageLayoutView="131" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A6" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,38 +1118,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="61"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="65" t="s">
+      <c r="H1" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="61"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="21" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="66" t="s">
+      <c r="H2" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1599,10 +1599,10 @@
       <c r="J19" s="38"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G20" s="67" t="s">
+      <c r="G20" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="67"/>
+      <c r="H20" s="54"/>
       <c r="I20" s="13">
         <f>SUM(I5:I19)</f>
         <v>62.5</v>
@@ -1617,101 +1617,101 @@
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="16"/>
-      <c r="G21" s="68" t="s">
+      <c r="G21" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="68"/>
+      <c r="H21" s="55"/>
       <c r="I21" s="11">
         <f>I20*0.19</f>
         <v>11.875</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="63"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="63" t="s">
+      <c r="D22" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="64"/>
-      <c r="G22" s="68" t="s">
+      <c r="E22" s="62"/>
+      <c r="G22" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="68"/>
+      <c r="H22" s="55"/>
       <c r="I22" s="12">
         <f>I20*1.19</f>
         <v>74.375</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="53"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="56" t="s">
+      <c r="D23" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="57"/>
+      <c r="E23" s="66"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="52" t="s">
+      <c r="A24" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="53"/>
+      <c r="B24" s="61"/>
       <c r="C24" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="56" t="s">
+      <c r="D24" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="57"/>
+      <c r="E24" s="66"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="53"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="56" t="s">
+      <c r="D25" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="57"/>
+      <c r="E25" s="66"/>
       <c r="H25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="53"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="56" t="s">
+      <c r="D26" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="57"/>
+      <c r="E26" s="66"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="55"/>
+      <c r="B27" s="64"/>
       <c r="C27" s="39"/>
-      <c r="D27" s="58" t="s">
+      <c r="D27" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="59"/>
+      <c r="E27" s="68"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="40" t="s">
@@ -1824,16 +1824,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D22:E22"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A27:B27"/>
@@ -1843,6 +1833,16 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>